<commit_message>
updates due to errors reported
</commit_message>
<xml_diff>
--- a/public/Enrollment.xlsx
+++ b/public/Enrollment.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="5010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="6990"/>
   </bookViews>
   <sheets>
     <sheet name="Batch_Enrolment" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>Program</t>
   </si>
@@ -45,15 +45,9 @@
     <t>Sub County</t>
   </si>
   <si>
-    <t>Facility</t>
-  </si>
-  <si>
     <t>MFL Code</t>
   </si>
   <si>
-    <t>Tester Name</t>
-  </si>
-  <si>
     <t>Tester Mobile Number</t>
   </si>
   <si>
@@ -72,9 +66,6 @@
     <t>Tester Address</t>
   </si>
   <si>
-    <t>Gender</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
@@ -253,6 +244,9 @@
   </si>
   <si>
     <t>RCO</t>
+  </si>
+  <si>
+    <t>Tester Unique ID</t>
   </si>
 </sst>
 </file>
@@ -260,7 +254,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0###\-###\-###"/>
+    <numFmt numFmtId="164" formatCode="0###\-###\-###"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -312,11 +306,11 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -621,34 +615,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.85546875" style="4"/>
+    <col min="3" max="3" width="11.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -659,86 +651,61 @@
         <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>11</v>
-      </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="MMRdUSeq1C+Ujao6aNO/I0RO8kT8XxkEVK4AHgYt2BWxjo+iKGCIvnF7iZCu+lbyA+GozxGbR60J/toxU+c5IA==" saltValue="GZYx+NfEOsxb30nyjcWPUA==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1" sort="0" autoFilter="0"/>
-  <dataValidations count="16">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Select gender from the list." sqref="F2:F1048576">
-      <formula1>Gender.</formula1>
-    </dataValidation>
+  <sheetProtection algorithmName="SHA-512" hashValue="i18GA6ec+hOWFB5oYY+TEH7X+7guKHuNd/XwFpvQmpCZB2IzZFl+CUoOHCWhZyJZREJE/erH+QV+hQ9yJDWJJQ==" saltValue="Uq1vDcwViZvB9LLa7U4Zyw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" sort="0" autoFilter="0"/>
+  <dataValidations count="10">
+    <dataValidation allowBlank="1" showInputMessage="1" errorTitle="Error" error="Select a county." sqref="A1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" errorTitle="Error" error="Select Designation" sqref="H1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" errorTitle="Error" error="Select Program" sqref="I1"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Select a county." sqref="A2:A1048576">
       <formula1>Counties.</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" errorTitle="Error" error="Select gender from the list." sqref="F1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" errorTitle="Error" error="Select a county." sqref="A1"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Select Designation" sqref="J2:J1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Select Designation" sqref="H2:H1048576">
       <formula1>Designations.</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" errorTitle="Error" error="Select Designation" sqref="J1"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Select Program" sqref="K2:K1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Select Program" sqref="I2:I1048576">
       <formula1>Programs.</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" errorTitle="Error" error="Select Program" sqref="K1"/>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Enter a valid email address." sqref="H1:H1048576 M1:M1048576">
-      <formula1>ISNUMBER(MATCH("*@*.???",H2,0))</formula1>
-    </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Enter a valid phone number." sqref="G1:G1048576">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Enter a valid phone number." sqref="E1:E1048576">
       <formula1>0</formula1>
       <formula2>9999999999</formula2>
-    </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Enter a valid MFL Code" sqref="D1:D1048576">
-      <formula1>1000</formula1>
-      <formula2>100000</formula2>
     </dataValidation>
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Enter a valid sub county." sqref="B1:B1048576">
       <formula1>4</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Enter a valid facility name." sqref="C1:C1048576">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Enter a valid name." sqref="J1:J1048576">
       <formula1>5</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Enter a valid tester name." sqref="E1:E1048576">
-      <formula1>5</formula1>
-      <formula2>100</formula2>
-    </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Enter a valid name." sqref="L1:L1048576">
-      <formula1>5</formula1>
-      <formula2>100</formula2>
-    </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N1:N1048576">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1:L1048576">
       <formula1>0</formula1>
       <formula2>9999999999</formula2>
     </dataValidation>
@@ -767,276 +734,276 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>